<commit_message>
Starting to implement javadoc Documentation
</commit_message>
<xml_diff>
--- a/Frogger/Testing report.xlsx
+++ b/Frogger/Testing report.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20088" windowHeight="4668" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20088" windowHeight="5832" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Iteratives Development Steps" sheetId="1" r:id="rId1"/>
     <sheet name="Testing Report" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <oleSize ref="A106:D115"/>
+  <oleSize ref="A1:D14"/>
 </workbook>
 </file>
 
@@ -801,7 +801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
@@ -1548,7 +1548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>

</xml_diff>